<commit_message>
Add screws and fuse to BOM
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -8,35 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCB0B71-F364-4012-9954-B14BC15F0A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02E2A01-FB51-4DE0-8B3B-CD2E417A3DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="242">
   <si>
     <t>Value</t>
   </si>
@@ -599,9 +588,6 @@
     <t>SUM non-brand stand and handle</t>
   </si>
   <si>
-    <t xml:space="preserve">non-brand Stand </t>
-  </si>
-  <si>
     <t>T210 handle piece + 3 tips</t>
   </si>
   <si>
@@ -717,6 +703,54 @@
   </si>
   <si>
     <t>AxxSolder V2.1</t>
+  </si>
+  <si>
+    <t>Fuse 10A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Littelfuse/0891005.NXS?qs=5b8eIUDTslk98GtnISs9VA%3D%3D</t>
+  </si>
+  <si>
+    <t>For the display</t>
+  </si>
+  <si>
+    <t>Screws - M3x8mm countersunk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the binder 99-0624-00-07 </t>
+  </si>
+  <si>
+    <t>Screws - M2.5x10mm</t>
+  </si>
+  <si>
+    <t>Screws - M2x8mm + nuts</t>
+  </si>
+  <si>
+    <t>For the aluminium rest</t>
+  </si>
+  <si>
+    <t>Aluminium plate 15x10x3 mm</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Station only</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Poratble only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-brand Stand </t>
+  </si>
+  <si>
+    <t>Connector for JBC stand (binder 99-0624-00-07)</t>
+  </si>
+  <si>
+    <t>https://de.farnell.com/binder/99-0624-00-07/socket-panelmontage-7pol/dp/1122418?pf_custSiteRedirect=true</t>
+  </si>
+  <si>
+    <t>Screws - M4x8mm</t>
+  </si>
+  <si>
+    <t>For enclosure to JBS stand</t>
   </si>
 </sst>
 </file>
@@ -727,7 +761,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,6 +816,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -804,24 +856,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -853,35 +905,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1166,164 +1248,151 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H63" sqref="A1:H63"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
     <col min="8" max="8" width="111" customWidth="1"/>
     <col min="9" max="9" width="100.42578125" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
     <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="17"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E4" s="7">
         <v>6</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F4" s="8">
         <v>0.89300000000000002</v>
       </c>
-      <c r="G3" s="12">
-        <f>E3*F3</f>
+      <c r="G4" s="9">
+        <f>E4*F4</f>
         <v>5.3580000000000005</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4" s="13">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G39" si="0">E4*F4</f>
-        <v>1.1160000000000001</v>
-      </c>
-      <c r="H4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
         <v>12</v>
       </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.88400000000000001</v>
+      <c r="F5" s="10">
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6520000000000001</v>
+        <f t="shared" ref="G5:G40" si="0">E5*F5</f>
+        <v>1.1160000000000001</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -1331,29 +1400,29 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="13">
-        <v>9.2999999999999999E-2</v>
+        <v>3</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.88400000000000001</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -1361,478 +1430,478 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1.1599999999999999</v>
+        <v>2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>1.1599999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="13">
-        <v>0.15</v>
+      <c r="F8" s="10">
+        <v>1.1599999999999999</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H8" t="s">
-        <v>215</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>216</v>
+        <v>136</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.26</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.15</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1.3</v>
+        <v>0.15</v>
       </c>
       <c r="H9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
+        <v>214</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0.41899999999999998</v>
+        <v>5</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.26</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0.41899999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="13">
-        <v>12.9</v>
+      <c r="F11" s="10">
+        <v>0.41899999999999998</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>12.9</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="13">
-        <v>0.44600000000000001</v>
+      <c r="F12" s="10">
+        <v>12.9</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>0.44600000000000001</v>
+        <v>12.9</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="13">
-        <v>0.58599999999999997</v>
+      <c r="F13" s="10">
+        <v>0.44600000000000001</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>0.58599999999999997</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="13">
-        <v>1.1000000000000001</v>
+      <c r="F14" s="10">
+        <v>0.58599999999999997</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="13">
-        <v>5.72</v>
+      <c r="F15" s="10">
+        <v>1.1000000000000001</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>5.72</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="13">
-        <v>6.45</v>
+      <c r="F16" s="10">
+        <v>5.72</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>6.45</v>
+        <v>5.72</v>
       </c>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>206</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>61</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="13">
-        <v>0.75</v>
+      <c r="F17" s="10">
+        <v>6.45</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>6.45</v>
       </c>
       <c r="H17" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="I17" t="s">
-        <v>208</v>
+        <v>62</v>
       </c>
       <c r="J17" t="s">
-        <v>205</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>209</v>
+        <v>59</v>
+      </c>
+      <c r="K17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>205</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="13">
-        <v>0.54900000000000004</v>
+      <c r="F18" s="10">
+        <v>0.75</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
-        <v>0.54900000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="H18" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="I18" t="s">
-        <v>68</v>
+        <v>207</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" t="s">
-        <v>69</v>
+        <v>204</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="13">
-        <v>3.78</v>
+      <c r="F19" s="10">
+        <v>0.54900000000000004</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="0"/>
-        <v>3.78</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="H19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="13">
-        <v>2.99</v>
+      <c r="F20" s="10">
+        <v>3.78</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>2.99</v>
+        <v>3.78</v>
       </c>
       <c r="H20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I20" t="s">
-        <v>8</v>
+        <v>74</v>
+      </c>
+      <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
@@ -1841,20 +1910,20 @@
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="13">
-        <v>1.5</v>
+      <c r="F21" s="10">
+        <v>2.99</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.99</v>
       </c>
       <c r="H21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I21" t="s">
         <v>8</v>
@@ -1862,181 +1931,181 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" s="13">
-        <v>2.71</v>
+      <c r="F22" s="10">
+        <v>1.5</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="0"/>
-        <v>2.71</v>
+        <v>1.5</v>
       </c>
       <c r="H22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I22" t="s">
-        <v>86</v>
-      </c>
-      <c r="J22" t="s">
-        <v>83</v>
-      </c>
-      <c r="K22" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" s="13">
-        <v>0.83699999999999997</v>
+      <c r="F23" s="10">
+        <v>2.71</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="0"/>
-        <v>0.83699999999999997</v>
+        <v>2.71</v>
       </c>
       <c r="H23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>200</v>
+        <v>91</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" s="13">
-        <v>1.84</v>
+      <c r="F24" s="10">
+        <v>0.83699999999999997</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="0"/>
-        <v>1.84</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="H24" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="I24" t="s">
-        <v>202</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>203</v>
+        <v>92</v>
+      </c>
+      <c r="J24" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="13">
-        <v>0.17699999999999999</v>
+      <c r="F25" s="10">
+        <v>1.84</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
-        <v>0.17699999999999999</v>
+        <v>1.84</v>
       </c>
       <c r="H25" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
-      </c>
-      <c r="J25" t="s">
-        <v>95</v>
-      </c>
-      <c r="K25" t="s">
-        <v>99</v>
+        <v>201</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E26">
-        <v>6</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0.36299999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.17699999999999999</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
-        <v>2.1779999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I26" t="s">
-        <v>8</v>
+        <v>98</v>
+      </c>
+      <c r="J26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
         <v>102</v>
@@ -2045,17 +2114,17 @@
         <v>103</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" s="13">
-        <v>0.186</v>
+        <v>6</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.36299999999999999</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
@@ -2063,10 +2132,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
         <v>102</v>
@@ -2077,15 +2146,15 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28" s="13">
-        <v>0.27</v>
+      <c r="F28" s="10">
+        <v>0.186</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.186</v>
       </c>
       <c r="H28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2093,10 +2162,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
         <v>102</v>
@@ -2105,17 +2174,17 @@
         <v>103</v>
       </c>
       <c r="E29">
-        <v>8</v>
-      </c>
-      <c r="F29" s="13">
-        <v>0.16700000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.27</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>
-        <v>1.3360000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2123,29 +2192,29 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
         <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30" s="13">
-        <v>0.92100000000000004</v>
+        <v>8</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.16700000000000001</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="0"/>
-        <v>0.92100000000000004</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="H30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2153,29 +2222,29 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31">
-        <v>220</v>
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
       </c>
       <c r="C31" t="s">
         <v>102</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="13">
-        <v>0.158</v>
+      <c r="F31" s="10">
+        <v>0.92100000000000004</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>0.158</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="H31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2183,10 +2252,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="B32" s="14">
+        <v>220</v>
       </c>
       <c r="C32" t="s">
         <v>102</v>
@@ -2195,17 +2264,17 @@
         <v>103</v>
       </c>
       <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="F32" s="13">
-        <v>0.17699999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.158</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
-        <v>0.35399999999999998</v>
+        <v>0.158</v>
       </c>
       <c r="H32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2213,10 +2282,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
         <v>102</v>
@@ -2227,15 +2296,15 @@
       <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33" s="13">
-        <v>9.2999999999999999E-2</v>
+      <c r="F33" s="10">
+        <v>0.17699999999999999</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2243,10 +2312,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>102</v>
@@ -2257,7 +2326,7 @@
       <c r="E34">
         <v>2</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="10">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G34" s="3">
@@ -2265,7 +2334,7 @@
         <v>0.186</v>
       </c>
       <c r="H34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2273,10 +2342,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>218</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>220</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
         <v>102</v>
@@ -2285,17 +2354,20 @@
         <v>103</v>
       </c>
       <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" s="13">
-        <v>0.09</v>
+        <v>2</v>
+      </c>
+      <c r="F35" s="10">
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>0.186</v>
       </c>
       <c r="H35" t="s">
-        <v>224</v>
+        <v>178</v>
+      </c>
+      <c r="I35" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2303,7 +2375,7 @@
         <v>217</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C36" t="s">
         <v>102</v>
@@ -2314,12 +2386,12 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36" s="13">
-        <v>0.16</v>
+      <c r="F36" s="10">
+        <v>0.09</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.09</v>
       </c>
       <c r="H36" t="s">
         <v>223</v>
@@ -2327,10 +2399,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C37" t="s">
         <v>102</v>
@@ -2341,399 +2413,559 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="13">
-        <v>0.09</v>
+      <c r="F37" s="10">
+        <v>0.16</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="H37" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>218</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="13">
-        <v>2.0699999999999998</v>
+      <c r="F38" s="10">
+        <v>0.09</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" si="0"/>
-        <v>2.0699999999999998</v>
+        <v>0.09</v>
       </c>
       <c r="H38" t="s">
-        <v>153</v>
-      </c>
-      <c r="I38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38" t="s">
-        <v>121</v>
-      </c>
-      <c r="K38" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="10">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H39" t="s">
+        <v>153</v>
+      </c>
+      <c r="I39" t="s">
+        <v>124</v>
+      </c>
+      <c r="J39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>126</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>127</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>128</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>128</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" s="13">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="10">
         <v>1.6</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G40" s="3">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="5">
-        <f>SUM(G3:G39)</f>
-        <v>64.461000000000013</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1" t="s">
+      <c r="G41" s="5">
+        <f>SUM(G4:G40)</f>
+        <v>64.461000000000013</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>155</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
-        <v>2</v>
-      </c>
-      <c r="G43" s="3">
-        <f>F43*E43</f>
-        <v>2</v>
-      </c>
-      <c r="H43" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" s="3">
-        <v>6.11</v>
+        <v>2</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" ref="G44:G48" si="1">F44*E44</f>
-        <v>6.11</v>
+        <f>F44*E44</f>
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>226</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="G45" s="3">
+        <f>F45*E45</f>
+        <v>0.38</v>
+      </c>
+      <c r="H45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="G46" s="3">
+        <f>F46*E46</f>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="H46" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>6.11</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" ref="G47:G56" si="1">F47*E47</f>
+        <v>6.11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>158</v>
       </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" s="3">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
         <v>2.12</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G48" s="3">
         <f t="shared" si="1"/>
         <v>2.12</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H48" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>182</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G49" s="3">
         <f t="shared" si="1"/>
         <v>2.0099999999999998</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H49" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G50" s="3">
         <f t="shared" si="1"/>
         <v>2.4700000000000002</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H50" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>160</v>
       </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" s="3">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
         <v>5</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G51" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="5">
-        <f>SUM(G43:G48)</f>
-        <v>19.71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B51" s="16"/>
+      <c r="H51" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" t="s">
+        <v>228</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" t="s">
+        <v>241</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G53" s="3">
+        <f>F52*E52</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B55" t="s">
+        <v>233</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="5">
+        <f>SUM(G44:G56)</f>
+        <v>27.599999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="12"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>163</v>
       </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="3">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
         <v>171.4</v>
       </c>
-      <c r="G52">
-        <f>F52*E52</f>
+      <c r="G60">
+        <f>F60*E60</f>
         <v>171.4</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H60" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>165</v>
       </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" s="3">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
         <v>66.34</v>
       </c>
-      <c r="G53">
-        <f t="shared" ref="G53:G54" si="2">F53*E53</f>
+      <c r="G61">
+        <f t="shared" ref="G61:G62" si="2">F61*E61</f>
         <v>66.34</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H61" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>169</v>
       </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="3">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
         <v>38.340000000000003</v>
       </c>
-      <c r="G54">
+      <c r="G62">
         <f t="shared" si="2"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H62" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
+    <row r="63" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G55" s="5">
-        <f>SUM(G52:G54)</f>
+      <c r="G63" s="5">
+        <f>SUM(G60:G62)</f>
         <v>276.08000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="16" t="s">
+    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="7" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="27"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>35.06</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ref="G66:G67" si="3">F66*E66</f>
+        <v>35.06</v>
+      </c>
+      <c r="H66" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>187</v>
       </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
-        <v>35.06</v>
-      </c>
-      <c r="G58">
-        <f t="shared" ref="G58:G59" si="3">F58*E58</f>
-        <v>35.06</v>
-      </c>
-      <c r="H58" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" s="3">
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3">
         <v>4.0199999999999996</v>
       </c>
-      <c r="G59">
+      <c r="G67">
         <f t="shared" si="3"/>
         <v>4.0199999999999996</v>
       </c>
-      <c r="H59" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A60" s="18" t="s">
+      <c r="H67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="G60" s="5">
-        <f>SUM(G58:G59)</f>
+      <c r="B68" s="13"/>
+      <c r="G68" s="5">
+        <f>SUM(G66:G67)</f>
         <v>39.08</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="17" t="s">
+    <row r="69" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="G62" s="6">
-        <f>G55+G49+G40</f>
-        <v>360.25100000000003</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="G63" s="8">
-        <f>G60+G49+G40</f>
-        <v>123.251</v>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="26">
+        <f>G63+G57+G41</f>
+        <v>368.14100000000008</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="26">
+        <f>G68+G57+G41</f>
+        <v>131.14100000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A60:B60"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H38" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H45" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H27" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H58" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H59" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H39" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H66" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H67" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="28" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
+  <pageSetup scale="26" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delete non-tested hardware (non-genuine JBC soldering iron)
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02E2A01-FB51-4DE0-8B3B-CD2E417A3DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757088B9-C7CC-44BB-8D28-3ABE3CBC40A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="240">
   <si>
     <t>Value</t>
   </si>
@@ -525,9 +525,6 @@
     <t>T210 handle piece</t>
   </si>
   <si>
-    <t>JBC stand and T210 handle piece</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/se/en/details/jbc-t210-a/soldering-stations-accessories/jbc-tools/t210-a/</t>
   </si>
   <si>
@@ -582,18 +579,6 @@
     <t>SUM JBC stand and handle</t>
   </si>
   <si>
-    <t>non-brand stand and T210 handle piece</t>
-  </si>
-  <si>
-    <t>SUM non-brand stand and handle</t>
-  </si>
-  <si>
-    <t>T210 handle piece + 3 tips</t>
-  </si>
-  <si>
-    <t>TOTAL Sum with non-brand handle and stand</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Price / component</t>
   </si>
   <si>
@@ -606,160 +591,170 @@
     <t>Prises as per 2023-10-03</t>
   </si>
   <si>
-    <t>WARNING: NOT tested, but does probably work</t>
+    <t>IC6</t>
+  </si>
+  <si>
+    <t>TPS54302DDCR</t>
+  </si>
+  <si>
+    <t>TPS54302DDCR:TPS54302DDCR</t>
+  </si>
+  <si>
+    <t>SOT95P280X110-6N</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Texas-Instruments/TPS54302DDCT?qs=zEmsApcVOkXGTx6CMk2KtQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=https://www.ti.com/lit/gpn/tps54302</t>
+  </si>
+  <si>
+    <t>TPS54302DDCT</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>SRP7028CC-100M</t>
+  </si>
+  <si>
+    <t>SRP7028CC-100M:SRP7028CC-100M</t>
+  </si>
+  <si>
+    <t>INDPM7366X300N</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRP7028CC.pdf</t>
+  </si>
+  <si>
+    <t>652-SRP7028CC-100M</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Bourns/SRP7028CC-100M?qs=1Kr7Jg1SGW%252BFrchEKUd2WQ%3D%3D</t>
+  </si>
+  <si>
+    <t>C1, C6, C12, C14, C19, C24</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>75p</t>
+  </si>
+  <si>
+    <t>C4, C17, C18, C25</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/KYOCERA-AVX/08051A750JAT2A?qs=xM%2FcMNU7BsFb8CFBKrIbNg%3D%3D</t>
+  </si>
+  <si>
+    <t>08051A750JAT2A</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>49.9</t>
+  </si>
+  <si>
+    <t>13k3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Vishay-Dale/RCC080549R9FKEA?qs=GedFDFLaBXFSdbXYm9WSig%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Bourns/CR0805AFX-1003ELF?qs=GedFDFLaBXEQCAFxmzLWkA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Bourns/CR0805-FX-1332ELF?qs=Hqdsf0hGw%2FBPaTV9GpndaQ%3D%3D</t>
+  </si>
+  <si>
+    <t>AxxSolder V2.1</t>
+  </si>
+  <si>
+    <t>Fuse 10A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Littelfuse/0891005.NXS?qs=5b8eIUDTslk98GtnISs9VA%3D%3D</t>
+  </si>
+  <si>
+    <t>For the display</t>
+  </si>
+  <si>
+    <t>Screws - M3x8mm countersunk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the binder 99-0624-00-07 </t>
+  </si>
+  <si>
+    <t>Screws - M2.5x10mm</t>
+  </si>
+  <si>
+    <t>Screws - M2x8mm + nuts</t>
+  </si>
+  <si>
+    <t>For the aluminium rest</t>
+  </si>
+  <si>
+    <t>Aluminium plate 15x10x3 mm</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Station only</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Poratble only</t>
+  </si>
+  <si>
+    <t>Connector for JBC stand (binder 99-0624-00-07)</t>
+  </si>
+  <si>
+    <t>https://de.farnell.com/binder/99-0624-00-07/socket-panelmontage-7pol/dp/1122418?pf_custSiteRedirect=true</t>
+  </si>
+  <si>
+    <t>Screws - M4x8mm</t>
+  </si>
+  <si>
+    <t>For enclosure to JBS stand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-brand Stand </t>
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005005857983522.html</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005005736571669.html</t>
-  </si>
-  <si>
-    <t>IC6</t>
-  </si>
-  <si>
-    <t>TPS54302DDCR</t>
-  </si>
-  <si>
-    <t>TPS54302DDCR:TPS54302DDCR</t>
-  </si>
-  <si>
-    <t>SOT95P280X110-6N</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Texas-Instruments/TPS54302DDCT?qs=zEmsApcVOkXGTx6CMk2KtQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=https://www.ti.com/lit/gpn/tps54302</t>
-  </si>
-  <si>
-    <t>TPS54302DDCT</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>SRP7028CC-100M</t>
-  </si>
-  <si>
-    <t>SRP7028CC-100M:SRP7028CC-100M</t>
-  </si>
-  <si>
-    <t>INDPM7366X300N</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRP7028CC.pdf</t>
-  </si>
-  <si>
-    <t>652-SRP7028CC-100M</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Bourns/SRP7028CC-100M?qs=1Kr7Jg1SGW%252BFrchEKUd2WQ%3D%3D</t>
-  </si>
-  <si>
-    <t>C1, C6, C12, C14, C19, C24</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>75p</t>
-  </si>
-  <si>
-    <t>C4, C17, C18, C25</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/KYOCERA-AVX/08051A750JAT2A?qs=xM%2FcMNU7BsFb8CFBKrIbNg%3D%3D</t>
-  </si>
-  <si>
-    <t>08051A750JAT2A</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>49.9</t>
-  </si>
-  <si>
-    <t>13k3</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Vishay-Dale/RCC080549R9FKEA?qs=GedFDFLaBXFSdbXYm9WSig%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Bourns/CR0805AFX-1003ELF?qs=GedFDFLaBXEQCAFxmzLWkA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Bourns/CR0805-FX-1332ELF?qs=Hqdsf0hGw%2FBPaTV9GpndaQ%3D%3D</t>
-  </si>
-  <si>
-    <t>AxxSolder V2.1</t>
-  </si>
-  <si>
-    <t>Fuse 10A</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/ProductDetail/Littelfuse/0891005.NXS?qs=5b8eIUDTslk98GtnISs9VA%3D%3D</t>
-  </si>
-  <si>
-    <t>For the display</t>
-  </si>
-  <si>
-    <t>Screws - M3x8mm countersunk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For the binder 99-0624-00-07 </t>
-  </si>
-  <si>
-    <t>Screws - M2.5x10mm</t>
-  </si>
-  <si>
-    <t>Screws - M2x8mm + nuts</t>
-  </si>
-  <si>
-    <t>For the aluminium rest</t>
-  </si>
-  <si>
-    <t>Aluminium plate 15x10x3 mm</t>
-  </si>
-  <si>
-    <t>Parts for AxxSolder Station only</t>
-  </si>
-  <si>
-    <t>Parts for AxxSolder Poratble only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-brand Stand </t>
-  </si>
-  <si>
-    <t>Connector for JBC stand (binder 99-0624-00-07)</t>
-  </si>
-  <si>
-    <t>https://de.farnell.com/binder/99-0624-00-07/socket-panelmontage-7pol/dp/1122418?pf_custSiteRedirect=true</t>
-  </si>
-  <si>
-    <t>Screws - M4x8mm</t>
-  </si>
-  <si>
-    <t>For enclosure to JBS stand</t>
+    <t>WARNING: NOT tested! Use at own risk</t>
+  </si>
+  <si>
+    <t>Non-genuine Stand</t>
+  </si>
+  <si>
+    <t>JBC stand</t>
+  </si>
+  <si>
+    <t>JBC T210 handle piece</t>
+  </si>
+  <si>
+    <t>TOTAL Sum with non-genuine JBC stand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -803,14 +798,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -828,6 +815,14 @@
     <font>
       <i/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -856,12 +851,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -869,6 +858,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -915,9 +910,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -926,21 +922,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -951,22 +945,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency 2" xfId="2" xr:uid="{B1965E38-26EB-4653-9601-BD7C1ADB6AF9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1248,10 +1243,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H71"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H71" sqref="A1:H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,29 +1266,29 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+        <v>217</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="17"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="22" t="s">
-        <v>236</v>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="14" t="s">
+        <v>228</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1320,10 +1315,10 @@
         <v>131</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
@@ -1337,36 +1332,36 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>6</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>0.89300000000000002</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <f>E4*F4</f>
         <v>5.3580000000000005</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1384,7 +1379,7 @@
       <c r="E5">
         <v>12</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G5" s="3">
@@ -1400,7 +1395,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1414,7 +1409,7 @@
       <c r="E6">
         <v>3</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.88400000000000001</v>
       </c>
       <c r="G6" s="3">
@@ -1444,7 +1439,7 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G7" s="3">
@@ -1474,7 +1469,7 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>1.1599999999999999</v>
       </c>
       <c r="G8" s="3">
@@ -1496,10 +1491,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1510,7 +1505,7 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>0.15</v>
       </c>
       <c r="G9" s="3">
@@ -1518,10 +1513,10 @@
         <v>0.15</v>
       </c>
       <c r="H9" t="s">
-        <v>214</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>215</v>
+        <v>206</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1540,7 +1535,7 @@
       <c r="E10">
         <v>5</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>0.26</v>
       </c>
       <c r="G10" s="3">
@@ -1570,7 +1565,7 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.41899999999999998</v>
       </c>
       <c r="G11" s="3">
@@ -1606,7 +1601,7 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>12.9</v>
       </c>
       <c r="G12" s="3">
@@ -1633,7 +1628,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>0.44600000000000001</v>
       </c>
       <c r="G13" s="3">
@@ -1669,7 +1664,7 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>0.58599999999999997</v>
       </c>
       <c r="G14" s="3">
@@ -1705,7 +1700,7 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="G15" s="3">
@@ -1735,7 +1730,7 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>5.72</v>
       </c>
       <c r="G16" s="3">
@@ -1771,7 +1766,7 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>6.45</v>
       </c>
       <c r="G17" s="3">
@@ -1793,21 +1788,21 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>0.75</v>
       </c>
       <c r="G18" s="3">
@@ -1815,16 +1810,16 @@
         <v>0.75</v>
       </c>
       <c r="H18" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I18" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="J18" t="s">
-        <v>204</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>208</v>
+        <v>196</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1843,7 +1838,7 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>0.54900000000000004</v>
       </c>
       <c r="G19" s="3">
@@ -1879,7 +1874,7 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>3.78</v>
       </c>
       <c r="G20" s="3">
@@ -1915,7 +1910,7 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>2.99</v>
       </c>
       <c r="G21" s="3">
@@ -1945,7 +1940,7 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>1.5</v>
       </c>
       <c r="G22" s="3">
@@ -1975,7 +1970,7 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>2.71</v>
       </c>
       <c r="G23" s="3">
@@ -2011,7 +2006,7 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <v>0.83699999999999997</v>
       </c>
       <c r="G24" s="3">
@@ -2033,21 +2028,21 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C25" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>1.84</v>
       </c>
       <c r="G25" s="3">
@@ -2055,13 +2050,13 @@
         <v>1.84</v>
       </c>
       <c r="H25" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I25" t="s">
-        <v>201</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>202</v>
+        <v>193</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2080,7 +2075,7 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="9">
         <v>0.17699999999999999</v>
       </c>
       <c r="G26" s="3">
@@ -2116,7 +2111,7 @@
       <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="9">
         <v>0.36299999999999999</v>
       </c>
       <c r="G27" s="3">
@@ -2124,7 +2119,7 @@
         <v>2.1779999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
@@ -2146,7 +2141,7 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="9">
         <v>0.186</v>
       </c>
       <c r="G28" s="3">
@@ -2154,7 +2149,7 @@
         <v>0.186</v>
       </c>
       <c r="H28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2176,7 +2171,7 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="9">
         <v>0.27</v>
       </c>
       <c r="G29" s="3">
@@ -2184,7 +2179,7 @@
         <v>0.27</v>
       </c>
       <c r="H29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2206,7 +2201,7 @@
       <c r="E30">
         <v>8</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="9">
         <v>0.16700000000000001</v>
       </c>
       <c r="G30" s="3">
@@ -2214,7 +2209,7 @@
         <v>1.3360000000000001</v>
       </c>
       <c r="H30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2236,7 +2231,7 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="9">
         <v>0.92100000000000004</v>
       </c>
       <c r="G31" s="3">
@@ -2244,7 +2239,7 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="H31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2254,7 +2249,7 @@
       <c r="A32" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="11">
         <v>220</v>
       </c>
       <c r="C32" t="s">
@@ -2266,7 +2261,7 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="9">
         <v>0.158</v>
       </c>
       <c r="G32" s="3">
@@ -2274,7 +2269,7 @@
         <v>0.158</v>
       </c>
       <c r="H32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2296,7 +2291,7 @@
       <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="9">
         <v>0.17699999999999999</v>
       </c>
       <c r="G33" s="3">
@@ -2304,7 +2299,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="H33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2326,7 +2321,7 @@
       <c r="E34">
         <v>2</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="9">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G34" s="3">
@@ -2334,7 +2329,7 @@
         <v>0.186</v>
       </c>
       <c r="H34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2356,7 +2351,7 @@
       <c r="E35">
         <v>2</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="9">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G35" s="3">
@@ -2364,7 +2359,7 @@
         <v>0.186</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -2372,10 +2367,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
         <v>102</v>
@@ -2386,7 +2381,7 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="9">
         <v>0.09</v>
       </c>
       <c r="G36" s="3">
@@ -2394,15 +2389,15 @@
         <v>0.09</v>
       </c>
       <c r="H36" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C37" t="s">
         <v>102</v>
@@ -2413,7 +2408,7 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="9">
         <v>0.16</v>
       </c>
       <c r="G37" s="3">
@@ -2421,15 +2416,15 @@
         <v>0.16</v>
       </c>
       <c r="H37" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
@@ -2440,7 +2435,7 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="9">
         <v>0.09</v>
       </c>
       <c r="G38" s="3">
@@ -2448,7 +2443,7 @@
         <v>0.09</v>
       </c>
       <c r="H38" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2467,7 +2462,7 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="9">
         <v>2.0699999999999998</v>
       </c>
       <c r="G39" s="3">
@@ -2503,7 +2498,7 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F40" s="9">
         <v>1.6</v>
       </c>
       <c r="G40" s="3">
@@ -2557,12 +2552,12 @@
         <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2575,12 +2570,12 @@
         <v>0.38</v>
       </c>
       <c r="H45" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>238</v>
+      <c r="A46" s="15" t="s">
+        <v>229</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -2593,11 +2588,11 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="H46" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E47">
@@ -2634,7 +2629,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2647,12 +2642,12 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="H49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
-        <v>180</v>
+      <c r="A50" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2665,7 +2660,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="H50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2683,15 +2678,15 @@
         <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -2703,13 +2698,16 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
+      <c r="H52" s="22" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
-        <v>240</v>
+      <c r="A53" s="15" t="s">
+        <v>231</v>
       </c>
       <c r="B53" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2721,13 +2719,16 @@
         <f>F52*E52</f>
         <v>0.4</v>
       </c>
+      <c r="H53" s="22" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>231</v>
+      <c r="A54" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="B54" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -2739,13 +2740,16 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
+      <c r="H54" s="22" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>232</v>
+      <c r="A55" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="B55" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -2757,10 +2761,13 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
+      <c r="H55" s="22" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>234</v>
+      <c r="A56" s="12" t="s">
+        <v>226</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2771,6 +2778,9 @@
       <c r="G56" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="H56" s="22" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -2788,171 +2798,156 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B59" s="12"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A59" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B59" s="21"/>
+    </row>
+    <row r="60" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" s="3">
+      <c r="E60" s="22">
+        <v>1</v>
+      </c>
+      <c r="F60" s="23">
         <v>171.4</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="22">
         <f>F60*E60</f>
         <v>171.4</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="22" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="23"/>
+    </row>
+    <row r="62" spans="1:8" s="22" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="21"/>
+      <c r="C62" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" s="27"/>
+    </row>
+    <row r="63" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" s="22">
+        <v>1</v>
+      </c>
+      <c r="F63" s="23">
+        <v>35.06</v>
+      </c>
+      <c r="G63" s="22">
+        <v>35.06</v>
+      </c>
+      <c r="H63" s="22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="23"/>
+    </row>
+    <row r="65" spans="1:8" s="22" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" s="21"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>165</v>
       </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="3">
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
         <v>66.34</v>
       </c>
-      <c r="G61">
-        <f t="shared" ref="G61:G62" si="2">F61*E61</f>
+      <c r="G66">
+        <f t="shared" ref="G66:G67" si="2">F66*E66</f>
         <v>66.34</v>
       </c>
-      <c r="H61" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>169</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" s="3">
+      <c r="H66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>168</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3">
         <v>38.340000000000003</v>
       </c>
-      <c r="G62">
+      <c r="G67">
         <f t="shared" si="2"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H62" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G63" s="5">
-        <f>SUM(G60:G62)</f>
-        <v>276.08000000000004</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D65" s="27"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>237</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" s="3">
-        <v>35.06</v>
-      </c>
-      <c r="G66">
-        <f t="shared" ref="G66:G67" si="3">F66*E66</f>
-        <v>35.06</v>
-      </c>
-      <c r="H66" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>187</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67" s="3">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="G67">
-        <f t="shared" si="3"/>
-        <v>4.0199999999999996</v>
-      </c>
       <c r="H67" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A68" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="B68" s="13"/>
+      <c r="A68" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="G68" s="5">
         <f>SUM(G66:G67)</f>
-        <v>39.08</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A69" s="4"/>
+        <v>104.68</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
+      <c r="A70" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
       <c r="G70" s="26">
-        <f>G63+G57+G41</f>
-        <v>368.14100000000008</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
+        <f>G68+G57+G41+G60</f>
+        <v>368.14100000000002</v>
+      </c>
+      <c r="H70" s="22"/>
+    </row>
+    <row r="71" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
       <c r="G71" s="26">
-        <f>G68+G57+G41</f>
-        <v>131.14100000000002</v>
-      </c>
+        <f>G68+G57+G41+G63</f>
+        <v>231.80100000000002</v>
+      </c>
+      <c r="H71" s="22"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2962,10 +2957,11 @@
     <hyperlink ref="H39" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="H48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="H28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H66" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H67" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H59" r:id="rId8" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H63" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H60" r:id="rId10" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="26" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
+  <pageSetup scale="26" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change capacitor to higher voltage rating
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757088B9-C7CC-44BB-8D28-3ABE3CBC40A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6424B09-8423-40B5-80C0-5501E3D5E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <t>https://www.mouser.se/ProductDetail/KYOCERA-AVX/KGM21NR71H104KT?qs=Jm2GQyTW%2Fbj%252BykwLLGtT1A%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.se/ProductDetail/KYOCERA-AVX/0805YC106KAT2A?qs=3HJ2avRr9PKwMzeRMZhF2g%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.se/ProductDetail/TDK/C3216X5R1V226M160AC?qs=NRhsANhppD8TwN31eZ1xGQ%3D%3D</t>
   </si>
   <si>
@@ -745,18 +742,20 @@
   </si>
   <si>
     <t>TOTAL Sum with non-genuine JBC stand</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Murata-Electronics/GRM21BR6YA106ME43L?qs=K0Sa7bCb58L8Cutg5cHuEA%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -827,6 +826,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -910,12 +918,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -936,6 +945,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -948,20 +965,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Currency 2" xfId="2" xr:uid="{B1965E38-26EB-4653-9601-BD7C1ADB6AF9}"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1243,10 +1254,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H71" sqref="A1:H71"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,15 +1276,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C1" s="18"/>
+      <c r="A1" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="24"/>
       <c r="D1" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -1284,11 +1295,11 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="17"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1315,10 +1326,10 @@
         <v>131</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
@@ -1333,7 +1344,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -1348,14 +1359,14 @@
         <v>6</v>
       </c>
       <c r="F4" s="7">
-        <v>0.89300000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="G4" s="8">
         <f>E4*F4</f>
-        <v>5.3580000000000005</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>133</v>
+        <v>1.92</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>239</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>8</v>
@@ -1386,7 +1397,7 @@
         <f t="shared" ref="G5:G40" si="0">E5*F5</f>
         <v>1.1160000000000001</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="28" t="s">
         <v>132</v>
       </c>
       <c r="I5" t="s">
@@ -1395,7 +1406,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1416,8 +1427,8 @@
         <f t="shared" si="0"/>
         <v>2.6520000000000001</v>
       </c>
-      <c r="H6" t="s">
-        <v>134</v>
+      <c r="H6" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -1446,8 +1457,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H7" t="s">
-        <v>135</v>
+      <c r="H7" s="26" t="s">
+        <v>134</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -1476,8 +1487,8 @@
         <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="H8" t="s">
-        <v>136</v>
+      <c r="H8" s="26" t="s">
+        <v>135</v>
       </c>
       <c r="I8" t="s">
         <v>19</v>
@@ -1491,10 +1502,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
         <v>203</v>
-      </c>
-      <c r="B9" t="s">
-        <v>204</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1512,11 +1523,11 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,8 +1553,8 @@
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="H10" t="s">
-        <v>137</v>
+      <c r="H10" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -1572,8 +1583,8 @@
         <f t="shared" si="0"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="H11" t="s">
-        <v>138</v>
+      <c r="H11" s="26" t="s">
+        <v>137</v>
       </c>
       <c r="I11" t="s">
         <v>30</v>
@@ -1608,8 +1619,8 @@
         <f t="shared" si="0"/>
         <v>12.9</v>
       </c>
-      <c r="H12" t="s">
-        <v>139</v>
+      <c r="H12" s="26" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1635,8 +1646,8 @@
         <f t="shared" si="0"/>
         <v>0.44600000000000001</v>
       </c>
-      <c r="H13" t="s">
-        <v>140</v>
+      <c r="H13" s="26" t="s">
+        <v>139</v>
       </c>
       <c r="I13" t="s">
         <v>40</v>
@@ -1671,8 +1682,8 @@
         <f t="shared" si="0"/>
         <v>0.58599999999999997</v>
       </c>
-      <c r="H14" t="s">
-        <v>141</v>
+      <c r="H14" s="26" t="s">
+        <v>140</v>
       </c>
       <c r="I14" t="s">
         <v>46</v>
@@ -1707,8 +1718,8 @@
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H15" t="s">
-        <v>142</v>
+      <c r="H15" s="26" t="s">
+        <v>141</v>
       </c>
       <c r="I15" t="s">
         <v>8</v>
@@ -1737,8 +1748,8 @@
         <f t="shared" si="0"/>
         <v>5.72</v>
       </c>
-      <c r="H16" t="s">
-        <v>143</v>
+      <c r="H16" s="26" t="s">
+        <v>142</v>
       </c>
       <c r="I16" t="s">
         <v>56</v>
@@ -1773,8 +1784,8 @@
         <f t="shared" si="0"/>
         <v>6.45</v>
       </c>
-      <c r="H17" t="s">
-        <v>144</v>
+      <c r="H17" s="26" t="s">
+        <v>143</v>
       </c>
       <c r="I17" t="s">
         <v>62</v>
@@ -1788,16 +1799,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" t="s">
         <v>195</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>196</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>197</v>
-      </c>
-      <c r="D18" t="s">
-        <v>198</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1809,17 +1820,17 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H18" t="s">
-        <v>201</v>
+      <c r="H18" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="I18" t="s">
+        <v>198</v>
+      </c>
+      <c r="J18" t="s">
+        <v>195</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="J18" t="s">
-        <v>196</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1845,8 +1856,8 @@
         <f t="shared" si="0"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="H19" t="s">
-        <v>145</v>
+      <c r="H19" s="26" t="s">
+        <v>144</v>
       </c>
       <c r="I19" t="s">
         <v>68</v>
@@ -1881,8 +1892,8 @@
         <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
-      <c r="H20" t="s">
-        <v>146</v>
+      <c r="H20" s="26" t="s">
+        <v>145</v>
       </c>
       <c r="I20" t="s">
         <v>74</v>
@@ -1917,8 +1928,8 @@
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="H21" t="s">
-        <v>147</v>
+      <c r="H21" s="26" t="s">
+        <v>146</v>
       </c>
       <c r="I21" t="s">
         <v>8</v>
@@ -1947,8 +1958,8 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H22" t="s">
-        <v>148</v>
+      <c r="H22" s="26" t="s">
+        <v>147</v>
       </c>
       <c r="I22" t="s">
         <v>8</v>
@@ -1977,8 +1988,8 @@
         <f t="shared" si="0"/>
         <v>2.71</v>
       </c>
-      <c r="H23" t="s">
-        <v>149</v>
+      <c r="H23" s="26" t="s">
+        <v>148</v>
       </c>
       <c r="I23" t="s">
         <v>86</v>
@@ -2013,8 +2024,8 @@
         <f t="shared" si="0"/>
         <v>0.83699999999999997</v>
       </c>
-      <c r="H24" t="s">
-        <v>150</v>
+      <c r="H24" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="I24" t="s">
         <v>92</v>
@@ -2028,16 +2039,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" t="s">
         <v>188</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>189</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>190</v>
-      </c>
-      <c r="D25" t="s">
-        <v>191</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2049,14 +2060,14 @@
         <f t="shared" si="0"/>
         <v>1.84</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" t="s">
         <v>192</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2082,8 +2093,8 @@
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="H26" t="s">
-        <v>151</v>
+      <c r="H26" s="26" t="s">
+        <v>150</v>
       </c>
       <c r="I26" t="s">
         <v>98</v>
@@ -2118,8 +2129,8 @@
         <f t="shared" si="0"/>
         <v>2.1779999999999999</v>
       </c>
-      <c r="H27" t="s">
-        <v>169</v>
+      <c r="H27" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
@@ -2148,8 +2159,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H28" t="s">
-        <v>170</v>
+      <c r="H28" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2178,8 +2189,8 @@
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="H29" t="s">
-        <v>171</v>
+      <c r="H29" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2208,8 +2219,8 @@
         <f t="shared" si="0"/>
         <v>1.3360000000000001</v>
       </c>
-      <c r="H30" t="s">
-        <v>172</v>
+      <c r="H30" s="26" t="s">
+        <v>171</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2238,8 +2249,8 @@
         <f t="shared" si="0"/>
         <v>0.92100000000000004</v>
       </c>
-      <c r="H31" t="s">
-        <v>173</v>
+      <c r="H31" s="26" t="s">
+        <v>172</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2268,8 +2279,8 @@
         <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
-      <c r="H32" t="s">
-        <v>174</v>
+      <c r="H32" s="26" t="s">
+        <v>173</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2298,8 +2309,8 @@
         <f t="shared" si="0"/>
         <v>0.35399999999999998</v>
       </c>
-      <c r="H33" t="s">
-        <v>175</v>
+      <c r="H33" s="26" t="s">
+        <v>174</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2328,8 +2339,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H34" t="s">
-        <v>176</v>
+      <c r="H34" s="26" t="s">
+        <v>175</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2358,8 +2369,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H35" t="s">
-        <v>177</v>
+      <c r="H35" s="26" t="s">
+        <v>176</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -2367,10 +2378,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C36" t="s">
         <v>102</v>
@@ -2388,16 +2399,16 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="H36" t="s">
-        <v>215</v>
+      <c r="H36" s="26" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C37" t="s">
         <v>102</v>
@@ -2415,16 +2426,16 @@
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="H37" t="s">
-        <v>214</v>
+      <c r="H37" s="26" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
@@ -2442,8 +2453,8 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="H38" t="s">
-        <v>216</v>
+      <c r="H38" s="26" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2469,8 +2480,8 @@
         <f t="shared" si="0"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="H39" t="s">
-        <v>153</v>
+      <c r="H39" s="26" t="s">
+        <v>152</v>
       </c>
       <c r="I39" t="s">
         <v>124</v>
@@ -2505,13 +2516,13 @@
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H40" t="s">
-        <v>152</v>
+      <c r="H40" s="26" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2520,7 +2531,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5">
         <f>SUM(G4:G40)</f>
-        <v>64.461000000000013</v>
+        <v>61.023000000000017</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
@@ -2534,12 +2545,12 @@
     </row>
     <row r="43" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2552,12 +2563,12 @@
         <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2569,13 +2580,13 @@
         <f>F45*E45</f>
         <v>0.38</v>
       </c>
-      <c r="H45" t="s">
-        <v>219</v>
+      <c r="H45" s="26" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -2587,13 +2598,13 @@
         <f>F46*E46</f>
         <v>5.1100000000000003</v>
       </c>
-      <c r="H46" t="s">
-        <v>230</v>
+      <c r="H46" s="26" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2605,13 +2616,13 @@
         <f t="shared" ref="G47:G56" si="1">F47*E47</f>
         <v>6.11</v>
       </c>
-      <c r="H47" t="s">
-        <v>156</v>
+      <c r="H47" s="26" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2623,13 +2634,13 @@
         <f t="shared" si="1"/>
         <v>2.12</v>
       </c>
-      <c r="H48" t="s">
-        <v>159</v>
+      <c r="H48" s="26" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2641,13 +2652,13 @@
         <f t="shared" si="1"/>
         <v>2.0099999999999998</v>
       </c>
-      <c r="H49" t="s">
-        <v>180</v>
+      <c r="H49" s="26" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2659,13 +2670,13 @@
         <f t="shared" si="1"/>
         <v>2.4700000000000002</v>
       </c>
-      <c r="H50" t="s">
-        <v>178</v>
+      <c r="H50" s="26" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -2678,15 +2689,15 @@
         <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -2698,16 +2709,16 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="H52" s="22" t="s">
-        <v>186</v>
+      <c r="H52" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B53" t="s">
         <v>231</v>
-      </c>
-      <c r="B53" t="s">
-        <v>232</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2719,16 +2730,16 @@
         <f>F52*E52</f>
         <v>0.4</v>
       </c>
-      <c r="H53" s="22" t="s">
-        <v>186</v>
+      <c r="H53" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -2740,16 +2751,16 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="H54" s="22" t="s">
-        <v>186</v>
+      <c r="H54" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B55" t="s">
         <v>224</v>
-      </c>
-      <c r="B55" t="s">
-        <v>225</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -2761,13 +2772,13 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H55" s="22" t="s">
-        <v>186</v>
+      <c r="H55" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2779,13 +2790,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H56" s="22" t="s">
-        <v>186</v>
+      <c r="H56" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2798,71 +2809,71 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="B59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="E60" s="22">
-        <v>1</v>
-      </c>
-      <c r="F60" s="23">
+      <c r="A59" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="20"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
         <v>171.4</v>
       </c>
-      <c r="G60" s="22">
+      <c r="G60">
         <f>F60*E60</f>
         <v>171.4</v>
       </c>
-      <c r="H60" s="22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F61" s="23"/>
-    </row>
-    <row r="62" spans="1:8" s="22" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="24" t="s">
+      <c r="H60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="D62" s="27"/>
-    </row>
-    <row r="63" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="B62" s="20"/>
+      <c r="C62" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D62" s="19"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>232</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
+        <v>35.06</v>
+      </c>
+      <c r="G63">
+        <v>35.06</v>
+      </c>
+      <c r="H63" t="s">
         <v>233</v>
       </c>
-      <c r="E63" s="22">
-        <v>1</v>
-      </c>
-      <c r="F63" s="23">
-        <v>35.06</v>
-      </c>
-      <c r="G63" s="22">
-        <v>35.06</v>
-      </c>
-      <c r="H63" s="22" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F64" s="23"/>
-    </row>
-    <row r="65" spans="1:8" s="22" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B65" s="21"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="20"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2875,12 +2886,12 @@
         <v>66.34</v>
       </c>
       <c r="H66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2893,12 +2904,12 @@
         <v>38.340000000000003</v>
       </c>
       <c r="H67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G68" s="5">
         <f>SUM(G66:G67)</f>
@@ -2906,60 +2917,55 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="26">
+      <c r="A70" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="18">
         <f>G68+G57+G41+G60</f>
-        <v>368.14100000000002</v>
-      </c>
-      <c r="H70" s="22"/>
+        <v>364.70300000000003</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="26">
+      <c r="A71" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="18">
         <f>G68+G57+G41+G63</f>
-        <v>231.80100000000002</v>
-      </c>
-      <c r="H71" s="22"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
+        <v>228.36300000000003</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H39" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H59" r:id="rId8" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H63" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H60" r:id="rId10" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
+    <hyperlink ref="H14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H48" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H28" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H59" r:id="rId7" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H63" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H60" r:id="rId9" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
+    <hyperlink ref="H7" r:id="rId10" xr:uid="{248762FA-4AB4-4C5B-BD9F-71361739AEC2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="26" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId11"/>

</xml_diff>

<commit_message>
Update connectors in BOM
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6424B09-8423-40B5-80C0-5501E3D5E2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8D80A-736F-4637-ADEA-FC2D0E678CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,12 +492,6 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>https://de.farnell.com/en-DE/binder/99-0624-00-07/socket-panel-7way/dp/1122418?ost=99+0624+00+07</t>
-  </si>
-  <si>
-    <t>Connector for soldering iron (binder 99-0624-00-07)</t>
-  </si>
-  <si>
     <t>Power connector (Anderson PP15)</t>
   </si>
   <si>
@@ -745,6 +739,12 @@
   </si>
   <si>
     <t>https://www.mouser.se/ProductDetail/Murata-Electronics/GRM21BR6YA106ME43L?qs=K0Sa7bCb58L8Cutg5cHuEA%3D%3D</t>
+  </si>
+  <si>
+    <t>Connector for soldering iron (HIROSE(HRS) RPC1-12RB-6P(71))</t>
+  </si>
+  <si>
+    <t>https://de.farnell.com/hirose-hrs/rpc1-12rb-6p-71/rundstecker-panelmontage-6pol/dp/1077728?pf_custSiteRedirect=true</t>
   </si>
 </sst>
 </file>
@@ -949,10 +949,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -965,9 +964,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1256,8 +1256,8 @@
   </sheetPr>
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,15 +1276,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="24"/>
+      <c r="A1" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="25"/>
       <c r="D1" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -1295,11 +1295,11 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1326,10 +1326,10 @@
         <v>131</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
@@ -1344,7 +1344,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -1365,8 +1365,8 @@
         <f>E4*F4</f>
         <v>1.92</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>239</v>
+      <c r="H4" s="21" t="s">
+        <v>237</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>8</v>
@@ -1397,7 +1397,7 @@
         <f t="shared" ref="G5:G40" si="0">E5*F5</f>
         <v>1.1160000000000001</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="22" t="s">
         <v>132</v>
       </c>
       <c r="I5" t="s">
@@ -1406,7 +1406,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1427,7 +1427,7 @@
         <f t="shared" si="0"/>
         <v>2.6520000000000001</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>133</v>
       </c>
       <c r="I6" t="s">
@@ -1457,7 +1457,7 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="20" t="s">
         <v>134</v>
       </c>
       <c r="I7" t="s">
@@ -1487,7 +1487,7 @@
         <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="20" t="s">
         <v>135</v>
       </c>
       <c r="I8" t="s">
@@ -1502,10 +1502,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1523,11 +1523,11 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="H9" s="26" t="s">
-        <v>205</v>
+      <c r="H9" s="20" t="s">
+        <v>203</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1553,7 +1553,7 @@
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="20" t="s">
         <v>136</v>
       </c>
       <c r="I10" t="s">
@@ -1583,7 +1583,7 @@
         <f t="shared" si="0"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="20" t="s">
         <v>137</v>
       </c>
       <c r="I11" t="s">
@@ -1619,7 +1619,7 @@
         <f t="shared" si="0"/>
         <v>12.9</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="20" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
         <f t="shared" si="0"/>
         <v>0.44600000000000001</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="20" t="s">
         <v>139</v>
       </c>
       <c r="I13" t="s">
@@ -1682,7 +1682,7 @@
         <f t="shared" si="0"/>
         <v>0.58599999999999997</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="20" t="s">
         <v>140</v>
       </c>
       <c r="I14" t="s">
@@ -1718,7 +1718,7 @@
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="20" t="s">
         <v>141</v>
       </c>
       <c r="I15" t="s">
@@ -1748,7 +1748,7 @@
         <f t="shared" si="0"/>
         <v>5.72</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="20" t="s">
         <v>142</v>
       </c>
       <c r="I16" t="s">
@@ -1784,7 +1784,7 @@
         <f t="shared" si="0"/>
         <v>6.45</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="20" t="s">
         <v>143</v>
       </c>
       <c r="I17" t="s">
@@ -1799,16 +1799,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" t="s">
         <v>194</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>195</v>
-      </c>
-      <c r="C18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D18" t="s">
-        <v>197</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1820,17 +1820,17 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H18" s="26" t="s">
-        <v>200</v>
+      <c r="H18" s="20" t="s">
+        <v>198</v>
       </c>
       <c r="I18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
         <f t="shared" si="0"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H19" s="20" t="s">
         <v>144</v>
       </c>
       <c r="I19" t="s">
@@ -1892,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="20" t="s">
         <v>145</v>
       </c>
       <c r="I20" t="s">
@@ -1928,7 +1928,7 @@
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="20" t="s">
         <v>146</v>
       </c>
       <c r="I21" t="s">
@@ -1958,7 +1958,7 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="20" t="s">
         <v>147</v>
       </c>
       <c r="I22" t="s">
@@ -1988,7 +1988,7 @@
         <f t="shared" si="0"/>
         <v>2.71</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="20" t="s">
         <v>148</v>
       </c>
       <c r="I23" t="s">
@@ -2024,7 +2024,7 @@
         <f t="shared" si="0"/>
         <v>0.83699999999999997</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="20" t="s">
         <v>149</v>
       </c>
       <c r="I24" t="s">
@@ -2039,16 +2039,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" t="s">
         <v>187</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>188</v>
-      </c>
-      <c r="C25" t="s">
-        <v>189</v>
-      </c>
-      <c r="D25" t="s">
-        <v>190</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2060,14 +2060,14 @@
         <f t="shared" si="0"/>
         <v>1.84</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="I25" t="s">
+        <v>190</v>
+      </c>
+      <c r="J25" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="I25" t="s">
-        <v>192</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2093,7 +2093,7 @@
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="20" t="s">
         <v>150</v>
       </c>
       <c r="I26" t="s">
@@ -2129,8 +2129,8 @@
         <f t="shared" si="0"/>
         <v>2.1779999999999999</v>
       </c>
-      <c r="H27" s="26" t="s">
-        <v>168</v>
+      <c r="H27" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
@@ -2159,8 +2159,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H28" s="26" t="s">
-        <v>169</v>
+      <c r="H28" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2189,8 +2189,8 @@
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="H29" s="26" t="s">
-        <v>170</v>
+      <c r="H29" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2219,8 +2219,8 @@
         <f t="shared" si="0"/>
         <v>1.3360000000000001</v>
       </c>
-      <c r="H30" s="26" t="s">
-        <v>171</v>
+      <c r="H30" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2249,8 +2249,8 @@
         <f t="shared" si="0"/>
         <v>0.92100000000000004</v>
       </c>
-      <c r="H31" s="26" t="s">
-        <v>172</v>
+      <c r="H31" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2279,8 +2279,8 @@
         <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
-      <c r="H32" s="26" t="s">
-        <v>173</v>
+      <c r="H32" s="20" t="s">
+        <v>171</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2309,8 +2309,8 @@
         <f t="shared" si="0"/>
         <v>0.35399999999999998</v>
       </c>
-      <c r="H33" s="26" t="s">
-        <v>174</v>
+      <c r="H33" s="20" t="s">
+        <v>172</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2339,8 +2339,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H34" s="26" t="s">
-        <v>175</v>
+      <c r="H34" s="20" t="s">
+        <v>173</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2369,8 +2369,8 @@
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="H35" s="26" t="s">
-        <v>176</v>
+      <c r="H35" s="20" t="s">
+        <v>174</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -2378,10 +2378,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" t="s">
         <v>208</v>
-      </c>
-      <c r="B36" t="s">
-        <v>210</v>
       </c>
       <c r="C36" t="s">
         <v>102</v>
@@ -2399,16 +2399,16 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="H36" s="26" t="s">
-        <v>214</v>
+      <c r="H36" s="20" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
         <v>102</v>
@@ -2426,16 +2426,16 @@
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="H37" s="26" t="s">
-        <v>213</v>
+      <c r="H37" s="20" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
@@ -2453,8 +2453,8 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="H38" s="26" t="s">
-        <v>215</v>
+      <c r="H38" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2480,7 +2480,7 @@
         <f t="shared" si="0"/>
         <v>2.0699999999999998</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="20" t="s">
         <v>152</v>
       </c>
       <c r="I39" t="s">
@@ -2516,7 +2516,7 @@
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H40" s="20" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="43" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2563,12 +2563,12 @@
         <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2580,14 +2580,15 @@
         <f>F45*E45</f>
         <v>0.38</v>
       </c>
-      <c r="H45" s="26" t="s">
-        <v>218</v>
+      <c r="H45" s="20" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>228</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B46" s="15"/>
       <c r="E46">
         <v>1</v>
       </c>
@@ -2598,14 +2599,15 @@
         <f>F46*E46</f>
         <v>5.1100000000000003</v>
       </c>
-      <c r="H46" s="26" t="s">
-        <v>229</v>
+      <c r="H46" s="20" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>156</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="B47" s="12"/>
       <c r="E47">
         <v>1</v>
       </c>
@@ -2616,13 +2618,13 @@
         <f t="shared" ref="G47:G56" si="1">F47*E47</f>
         <v>6.11</v>
       </c>
-      <c r="H47" s="26" t="s">
-        <v>155</v>
+      <c r="H47" s="20" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2634,13 +2636,13 @@
         <f t="shared" si="1"/>
         <v>2.12</v>
       </c>
-      <c r="H48" s="26" t="s">
-        <v>158</v>
+      <c r="H48" s="20" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2652,13 +2654,13 @@
         <f t="shared" si="1"/>
         <v>2.0099999999999998</v>
       </c>
-      <c r="H49" s="26" t="s">
-        <v>179</v>
+      <c r="H49" s="20" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -2670,13 +2672,13 @@
         <f t="shared" si="1"/>
         <v>2.4700000000000002</v>
       </c>
-      <c r="H50" s="26" t="s">
-        <v>177</v>
+      <c r="H50" s="20" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -2689,15 +2691,15 @@
         <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -2710,15 +2712,15 @@
         <v>0.4</v>
       </c>
       <c r="H52" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2731,15 +2733,15 @@
         <v>0.4</v>
       </c>
       <c r="H53" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -2752,15 +2754,15 @@
         <v>0.4</v>
       </c>
       <c r="H54" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -2773,12 +2775,12 @@
         <v>0.2</v>
       </c>
       <c r="H55" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2791,12 +2793,12 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2809,14 +2811,14 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B59" s="20"/>
+      <c r="A59" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="27"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2829,25 +2831,25 @@
         <v>171.4</v>
       </c>
       <c r="H60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B62" s="20"/>
+      <c r="A62" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B62" s="27"/>
       <c r="C62" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2859,21 +2861,21 @@
         <v>35.06</v>
       </c>
       <c r="H63" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="B65" s="20"/>
+      <c r="A65" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="B65" s="27"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2886,12 +2888,12 @@
         <v>66.34</v>
       </c>
       <c r="H66" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2904,12 +2906,12 @@
         <v>38.340000000000003</v>
       </c>
       <c r="H67" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G68" s="5">
         <f>SUM(G66:G67)</f>
@@ -2917,11 +2919,11 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
+      <c r="A70" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
@@ -2931,11 +2933,11 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
+      <c r="A71" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
@@ -2946,14 +2948,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A65:B65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
Fix output voltage from DC/DC by switching values of R28 and R27. Also change value of C24
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A8D80A-736F-4637-ADEA-FC2D0E678CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A62C3-564B-4D7A-A3E2-F30AADB6039C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="242">
   <si>
     <t>Value</t>
   </si>
@@ -54,9 +54,6 @@
     <t>~</t>
   </si>
   <si>
-    <t>C2, C3, C5, C7, C8, C9, C10, C11, C13, C20, C21, C22</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -492,12 +489,6 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>Power connector (Anderson PP15)</t>
-  </si>
-  <si>
-    <t>https://www.mouser.se/c/?marcom=154437221</t>
-  </si>
-  <si>
     <t>3D printed housing</t>
   </si>
   <si>
@@ -624,9 +615,6 @@
     <t>https://www.mouser.se/ProductDetail/Bourns/SRP7028CC-100M?qs=1Kr7Jg1SGW%252BFrchEKUd2WQ%3D%3D</t>
   </si>
   <si>
-    <t>C1, C6, C12, C14, C19, C24</t>
-  </si>
-  <si>
     <t>C26</t>
   </si>
   <si>
@@ -669,9 +657,6 @@
     <t>https://www.mouser.se/ProductDetail/Bourns/CR0805-FX-1332ELF?qs=Hqdsf0hGw%2FBPaTV9GpndaQ%3D%3D</t>
   </si>
   <si>
-    <t>AxxSolder V2.1</t>
-  </si>
-  <si>
     <t>Fuse 10A</t>
   </si>
   <si>
@@ -745,6 +730,27 @@
   </si>
   <si>
     <t>https://de.farnell.com/hirose-hrs/rpc1-12rb-6p-71/rundstecker-panelmontage-6pol/dp/1077728?pf_custSiteRedirect=true</t>
+  </si>
+  <si>
+    <t>C1, C6, C12, C14, C19</t>
+  </si>
+  <si>
+    <t>C2, C3, C5, C7, C8, C9, C10, C11, C13, C20, C21, C22, C24</t>
+  </si>
+  <si>
+    <t>Power connector (Anderson PP30) RED</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Anderson-Power-Products/1330G4?qs=yoCgdRjoRtEz6n6mDpzjEQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/Anderson-Power-Products/1330?qs=yoCgdRjoRtExZTZ%2Fg8W40Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Power connector (Anderson PP30)BLACK</t>
+  </si>
+  <si>
+    <t>AxxSolder V2.1 - REV B</t>
   </si>
 </sst>
 </file>
@@ -924,7 +930,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -952,6 +958,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -964,10 +974,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1254,15 +1261,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
@@ -1276,15 +1283,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="25"/>
+      <c r="A1" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="27"/>
       <c r="D1" s="12" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -1295,11 +1302,11 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="14" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1311,25 +1318,25 @@
     </row>
     <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
@@ -1344,7 +1351,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -1356,17 +1363,17 @@
         <v>7</v>
       </c>
       <c r="E4" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="7">
         <v>0.32</v>
       </c>
       <c r="G4" s="8">
         <f>E4*F4</f>
-        <v>1.92</v>
+        <v>1.6</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>8</v>
@@ -1376,10 +1383,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1388,17 +1395,17 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="9">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ref="G5:G40" si="0">E5*F5</f>
-        <v>1.1160000000000001</v>
+        <v>1.2090000000000001</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -1406,16 +1413,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1428,7 +1435,7 @@
         <v>2.6520000000000001</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -1436,10 +1443,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1458,7 +1465,7 @@
         <v>0.186</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -1466,16 +1473,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1488,24 +1495,24 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1524,24 +1531,24 @@
         <v>0.15</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1554,7 +1561,7 @@
         <v>1.3</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -1562,16 +1569,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1584,30 +1591,30 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
         <v>30</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>31</v>
-      </c>
-      <c r="K11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1620,21 +1627,21 @@
         <v>12.9</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1647,30 +1654,30 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" t="s">
         <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1683,30 +1690,30 @@
         <v>0.58599999999999997</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" t="s">
         <v>46</v>
-      </c>
-      <c r="J14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1719,7 +1726,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I15" t="s">
         <v>8</v>
@@ -1727,16 +1734,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>53</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1749,30 +1756,30 @@
         <v>5.72</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s">
         <v>56</v>
-      </c>
-      <c r="J16" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1785,30 +1792,30 @@
         <v>6.45</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" t="s">
         <v>62</v>
-      </c>
-      <c r="J17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" t="s">
         <v>192</v>
-      </c>
-      <c r="B18" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D18" t="s">
-        <v>195</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1821,30 +1828,30 @@
         <v>0.75</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I18" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1857,30 +1864,30 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" t="s">
         <v>68</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1893,30 +1900,30 @@
         <v>3.78</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" t="s">
         <v>74</v>
-      </c>
-      <c r="J20" t="s">
-        <v>71</v>
-      </c>
-      <c r="K20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
         <v>76</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>77</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1929,7 +1936,7 @@
         <v>2.99</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I21" t="s">
         <v>8</v>
@@ -1937,16 +1944,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
         <v>80</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1959,7 +1966,7 @@
         <v>1.5</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I22" t="s">
         <v>8</v>
@@ -1967,16 +1974,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>85</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1989,30 +1996,30 @@
         <v>2.71</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" t="s">
         <v>86</v>
-      </c>
-      <c r="J23" t="s">
-        <v>83</v>
-      </c>
-      <c r="K23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" t="s">
-        <v>91</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2025,30 +2032,30 @@
         <v>0.83699999999999997</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I24" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" t="s">
         <v>92</v>
-      </c>
-      <c r="J24" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" t="s">
         <v>185</v>
-      </c>
-      <c r="B25" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" t="s">
-        <v>188</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2061,27 +2068,27 @@
         <v>1.84</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
         <v>94</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>95</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" t="s">
-        <v>97</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -2094,30 +2101,30 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I26" t="s">
+        <v>97</v>
+      </c>
+      <c r="J26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K26" t="s">
         <v>98</v>
-      </c>
-      <c r="J26" t="s">
-        <v>95</v>
-      </c>
-      <c r="K26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
         <v>100</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
       </c>
       <c r="E27">
         <v>6</v>
@@ -2130,7 +2137,7 @@
         <v>2.1779999999999999</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I27" t="s">
         <v>8</v>
@@ -2138,16 +2145,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
         <v>104</v>
       </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
       <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
         <v>102</v>
-      </c>
-      <c r="D28" t="s">
-        <v>103</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -2160,7 +2167,7 @@
         <v>0.186</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2168,16 +2175,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
         <v>106</v>
       </c>
-      <c r="B29" t="s">
-        <v>107</v>
-      </c>
       <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
         <v>102</v>
-      </c>
-      <c r="D29" t="s">
-        <v>103</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2190,7 +2197,7 @@
         <v>0.27</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2198,16 +2205,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
         <v>108</v>
       </c>
-      <c r="B30" t="s">
-        <v>109</v>
-      </c>
       <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
         <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
       </c>
       <c r="E30">
         <v>8</v>
@@ -2220,7 +2227,7 @@
         <v>1.3360000000000001</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2228,16 +2235,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
         <v>110</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
         <v>111</v>
-      </c>
-      <c r="C31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" t="s">
-        <v>112</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -2250,7 +2257,7 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2258,16 +2265,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="11">
         <v>220</v>
       </c>
       <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
         <v>102</v>
-      </c>
-      <c r="D32" t="s">
-        <v>103</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2280,7 +2287,7 @@
         <v>0.158</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2288,16 +2295,16 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
         <v>114</v>
       </c>
-      <c r="B33" t="s">
-        <v>115</v>
-      </c>
       <c r="C33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" t="s">
         <v>102</v>
-      </c>
-      <c r="D33" t="s">
-        <v>103</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -2310,7 +2317,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2318,16 +2325,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
-        <v>117</v>
-      </c>
       <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>103</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -2340,7 +2347,7 @@
         <v>0.186</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2348,16 +2355,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
         <v>118</v>
       </c>
-      <c r="B35" t="s">
-        <v>119</v>
-      </c>
       <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
         <v>102</v>
-      </c>
-      <c r="D35" t="s">
-        <v>103</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -2370,7 +2377,7 @@
         <v>0.186</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -2378,70 +2385,70 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" t="s">
         <v>102</v>
       </c>
-      <c r="D36" t="s">
-        <v>103</v>
-      </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" s="9">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="0"/>
-        <v>0.09</v>
+        <f>E36*F36</f>
+        <v>0.16</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" t="s">
         <v>102</v>
       </c>
-      <c r="D37" t="s">
-        <v>103</v>
-      </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" s="9">
-        <v>0.16</v>
+        <v>0.09</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>E37*F37</f>
+        <v>0.09</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
         <v>102</v>
-      </c>
-      <c r="D38" t="s">
-        <v>103</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2454,21 +2461,21 @@
         <v>0.09</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" t="s">
         <v>120</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>121</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>122</v>
-      </c>
-      <c r="D39" t="s">
-        <v>123</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2481,30 +2488,30 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I39" t="s">
+        <v>123</v>
+      </c>
+      <c r="J39" t="s">
+        <v>120</v>
+      </c>
+      <c r="K39" t="s">
         <v>124</v>
-      </c>
-      <c r="J39" t="s">
-        <v>121</v>
-      </c>
-      <c r="K39" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
         <v>126</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>127</v>
       </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
       <c r="D40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2517,12 +2524,12 @@
         <v>1.6</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2531,7 +2538,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="5">
         <f>SUM(G4:G40)</f>
-        <v>61.023000000000017</v>
+        <v>60.796000000000014</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
@@ -2545,12 +2552,12 @@
     </row>
     <row r="43" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2563,12 +2570,12 @@
         <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2581,12 +2588,12 @@
         <v>0.38</v>
       </c>
       <c r="H45" s="20" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B46" s="15"/>
       <c r="E46">
@@ -2600,12 +2607,12 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B47" s="12"/>
       <c r="E47">
@@ -2615,361 +2622,379 @@
         <v>6.11</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" ref="G47:G56" si="1">F47*E47</f>
+        <f>F47*E47</f>
         <v>6.11</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>155</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="B48" s="29"/>
       <c r="E48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" s="3">
-        <v>2.12</v>
+        <v>1.22</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" si="1"/>
-        <v>2.12</v>
+        <f t="shared" ref="G48:G50" si="1">F48*E48</f>
+        <v>2.44</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>156</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49" s="3">
-        <v>2.0099999999999998</v>
+        <v>1.22</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" si="1"/>
+        <v>2.44</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
         <v>2.0099999999999998</v>
-      </c>
-      <c r="H49" s="20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3">
-        <v>2.4700000000000002</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" si="1"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="H50" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="H50" s="20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3">
-        <v>5</v>
-      </c>
       <c r="G51" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H51" t="s">
-        <v>183</v>
+        <f t="shared" ref="G47:G57" si="2">F51*E51</f>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>218</v>
-      </c>
-      <c r="B52" t="s">
-        <v>217</v>
+        <v>154</v>
       </c>
       <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>5</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" t="s">
+        <v>212</v>
+      </c>
+      <c r="E53">
         <v>4</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F53" s="3">
         <v>0.1</v>
       </c>
-      <c r="G52" s="3">
-        <f t="shared" si="1"/>
+      <c r="G53" s="3">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="H52" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B53" t="s">
-        <v>229</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" s="3">
+      <c r="H53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
         <v>0.2</v>
       </c>
-      <c r="G53" s="3">
-        <f>F52*E52</f>
+      <c r="G54" s="3">
+        <f>F53*E53</f>
         <v>0.4</v>
       </c>
-      <c r="H53" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B54" t="s">
-        <v>219</v>
-      </c>
-      <c r="E54">
-        <v>4</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G54" s="3">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
       <c r="H54" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F55" s="3">
         <v>0.1</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f t="shared" si="2"/>
+        <v>0.4</v>
       </c>
       <c r="H55" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="B56" t="s">
+        <v>217</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F56" s="3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="H56" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="5">
+        <f>SUM(G44:G57)</f>
+        <v>30.359999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B60" s="24"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>171.4</v>
+      </c>
+      <c r="G61">
+        <f>F61*E61</f>
+        <v>171.4</v>
+      </c>
+      <c r="H61" t="s">
         <v>158</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="5">
-        <f>SUM(G44:G56)</f>
-        <v>27.599999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="B59" s="27"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" s="3">
-        <v>171.4</v>
-      </c>
-      <c r="G60">
-        <f>F60*E60</f>
-        <v>171.4</v>
-      </c>
-      <c r="H60" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="B62" s="27"/>
-      <c r="C62" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D62" s="19"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D63" s="19"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>225</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3">
+        <v>35.06</v>
+      </c>
+      <c r="G64">
+        <v>35.06</v>
+      </c>
+      <c r="H64" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63" s="3">
-        <v>35.06</v>
-      </c>
-      <c r="G63">
-        <v>35.06</v>
-      </c>
-      <c r="H63" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="B65" s="27"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" s="3">
-        <v>66.34</v>
-      </c>
-      <c r="G66">
-        <f t="shared" ref="G66:G67" si="2">F66*E66</f>
-        <v>66.34</v>
-      </c>
-      <c r="H66" t="s">
-        <v>163</v>
-      </c>
+      <c r="B66" s="24"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67" s="3">
+        <v>66.34</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G68" si="3">F67*E67</f>
+        <v>66.34</v>
+      </c>
+      <c r="H67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>162</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
         <v>38.340000000000003</v>
       </c>
-      <c r="G67">
-        <f t="shared" si="2"/>
+      <c r="G68">
+        <f t="shared" si="3"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H67" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G68" s="5">
-        <f>SUM(G66:G67)</f>
+      <c r="H68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G69" s="5">
+        <f>SUM(G67:G68)</f>
         <v>104.68</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="18">
-        <f>G68+G57+G41+G60</f>
-        <v>364.70300000000003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
+    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
       <c r="G71" s="18">
-        <f>G68+G57+G41+G63</f>
-        <v>228.36300000000003</v>
+        <f>G69+G58+G41+G61</f>
+        <v>367.23599999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="18">
+        <f>G69+G58+G41+G64</f>
+        <v>230.89600000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A70:C70"/>
     <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A63:B63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="H16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="H19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="H39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H48" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H28" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H59" r:id="rId7" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H63" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H60" r:id="rId9" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
-    <hyperlink ref="H7" r:id="rId10" xr:uid="{248762FA-4AB4-4C5B-BD9F-71361739AEC2}"/>
+    <hyperlink ref="H28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H60" r:id="rId6" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H64" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H61" r:id="rId8" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
+    <hyperlink ref="H7" r:id="rId9" xr:uid="{248762FA-4AB4-4C5B-BD9F-71361739AEC2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="26" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId11"/>
+  <pageSetup scale="25" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update BOM with C25 to be a 0805 Capacitor
</commit_message>
<xml_diff>
--- a/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
+++ b/PCB/AxxSolder/bom/BOM_AxxSolder_V2_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\ownCloud - axel@192.168.1.36\2_Project\00_AxxProjects\AxxSolder\PCB\AxxSolder\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axel_\Desktop\AxxSolder\PCB\AxxSolder\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A62C3-564B-4D7A-A3E2-F30AADB6039C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6BCB75-B312-4D2E-A814-483B73C8616A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="244">
   <si>
     <t>Value</t>
   </si>
@@ -621,9 +621,6 @@
     <t>75p</t>
   </si>
   <si>
-    <t>C4, C17, C18, C25</t>
-  </si>
-  <si>
     <t>https://www.mouser.se/ProductDetail/KYOCERA-AVX/08051A750JAT2A?qs=xM%2FcMNU7BsFb8CFBKrIbNg%3D%3D</t>
   </si>
   <si>
@@ -751,6 +748,15 @@
   </si>
   <si>
     <t>AxxSolder V2.1 - REV B</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>https://www.mouser.se/ProductDetail/TDK/C2012X6S1C226M125AC?qs=6JAMGB%252BEdkzwYUkuPLa%252B7A%3D%3D</t>
+  </si>
+  <si>
+    <t>C4, C17, C18</t>
   </si>
 </sst>
 </file>
@@ -930,7 +936,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -974,7 +980,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1261,10 +1266,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,14 +1289,14 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>181</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -1306,7 +1311,7 @@
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1351,7 +1356,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -1373,7 +1378,7 @@
         <v>1.6</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>8</v>
@@ -1383,7 +1388,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1401,7 +1406,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G40" si="0">E5*F5</f>
+        <f t="shared" ref="G5:G41" si="0">E5*F5</f>
         <v>1.2090000000000001</v>
       </c>
       <c r="H5" s="22" t="s">
@@ -1413,7 +1418,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1443,10 +1448,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1455,496 +1460,493 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="9">
-        <v>9.2999999999999999E-2</v>
+        <v>0.54</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>0.54</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="9">
-        <v>1.1599999999999999</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>1.1599999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" s="9">
-        <v>0.15</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>200</v>
+        <v>134</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10" s="9">
-        <v>0.26</v>
+        <v>0.15</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1.3</v>
+        <v>0.15</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="I10" t="s">
-        <v>8</v>
+        <v>198</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" s="9">
-        <v>0.41899999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0.41899999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" s="9">
-        <v>12.9</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>12.9</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" s="9">
-        <v>0.44600000000000001</v>
+        <v>12.9</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>0.44600000000000001</v>
+        <v>12.9</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="I13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" s="9">
-        <v>0.58599999999999997</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>0.58599999999999997</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="9">
-        <v>1.1000000000000001</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I15" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="9">
-        <v>5.72</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>5.72</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" s="9">
-        <v>6.45</v>
+        <v>5.72</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>6.45</v>
+        <v>5.72</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" s="9">
-        <v>0.75</v>
+        <v>6.45</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>6.45</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
       <c r="I18" t="s">
-        <v>193</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>190</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>194</v>
+        <v>58</v>
+      </c>
+      <c r="K18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" s="9">
-        <v>0.54900000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="0"/>
-        <v>0.54900000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K19" t="s">
-        <v>68</v>
+        <v>190</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" s="9">
-        <v>3.78</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>3.78</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" s="9">
-        <v>2.99</v>
+        <v>3.78</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="0"/>
-        <v>2.99</v>
+        <v>3.78</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I21" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
@@ -1953,20 +1955,20 @@
         <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" s="9">
-        <v>1.5</v>
+        <v>2.99</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.99</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I22" t="s">
         <v>8</v>
@@ -1974,181 +1976,181 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" s="9">
-        <v>2.71</v>
+        <v>1.5</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="0"/>
-        <v>2.71</v>
+        <v>1.5</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J23" t="s">
-        <v>82</v>
-      </c>
-      <c r="K23" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" s="9">
-        <v>0.83699999999999997</v>
+        <v>2.71</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="0"/>
-        <v>0.83699999999999997</v>
+        <v>2.71</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" s="9">
-        <v>1.84</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
-        <v>1.84</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="I25" t="s">
-        <v>187</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>188</v>
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>184</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" s="9">
-        <v>0.17699999999999999</v>
+        <v>1.84</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
-        <v>0.17699999999999999</v>
+        <v>1.84</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="I26" t="s">
-        <v>97</v>
-      </c>
-      <c r="J26" t="s">
-        <v>94</v>
-      </c>
-      <c r="K26" t="s">
-        <v>98</v>
+        <v>187</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F27" s="9">
-        <v>0.36299999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
-        <v>2.1779999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="I27" t="s">
-        <v>8</v>
+        <v>97</v>
+      </c>
+      <c r="J27" t="s">
+        <v>94</v>
+      </c>
+      <c r="K27" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
         <v>101</v>
@@ -2157,17 +2159,17 @@
         <v>102</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F28" s="9">
-        <v>0.186</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I28" t="s">
         <v>8</v>
@@ -2175,10 +2177,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>101</v>
@@ -2190,14 +2192,14 @@
         <v>1</v>
       </c>
       <c r="F29" s="9">
-        <v>0.27</v>
+        <v>0.186</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.186</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I29" t="s">
         <v>8</v>
@@ -2205,10 +2207,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
         <v>101</v>
@@ -2217,17 +2219,17 @@
         <v>102</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F30" s="9">
-        <v>0.16700000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="0"/>
-        <v>1.3360000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I30" t="s">
         <v>8</v>
@@ -2235,29 +2237,29 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
         <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F31" s="9">
-        <v>0.92100000000000004</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>0.92100000000000004</v>
+        <v>1.3360000000000001</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I31" t="s">
         <v>8</v>
@@ -2265,29 +2267,29 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="11">
-        <v>220</v>
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
       </c>
       <c r="C32" t="s">
         <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" s="9">
-        <v>0.158</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
-        <v>0.158</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I32" t="s">
         <v>8</v>
@@ -2295,10 +2297,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
-      </c>
-      <c r="B33" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="B33" s="11">
+        <v>220</v>
       </c>
       <c r="C33" t="s">
         <v>101</v>
@@ -2307,17 +2309,17 @@
         <v>102</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" s="9">
-        <v>0.17699999999999999</v>
+        <v>0.158</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="0"/>
-        <v>0.35399999999999998</v>
+        <v>0.158</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
@@ -2325,10 +2327,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
         <v>101</v>
@@ -2340,14 +2342,14 @@
         <v>2</v>
       </c>
       <c r="F34" s="9">
-        <v>9.2999999999999999E-2</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="0"/>
-        <v>0.186</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I34" t="s">
         <v>8</v>
@@ -2355,10 +2357,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s">
         <v>101</v>
@@ -2377,7 +2379,7 @@
         <v>0.186</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I35" t="s">
         <v>8</v>
@@ -2385,10 +2387,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
         <v>101</v>
@@ -2397,17 +2399,20 @@
         <v>102</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" s="9">
-        <v>0.16</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G36" s="3">
-        <f>E36*F36</f>
-        <v>0.16</v>
+        <f t="shared" si="0"/>
+        <v>0.186</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>207</v>
+        <v>171</v>
+      </c>
+      <c r="I36" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2427,22 +2432,22 @@
         <v>1</v>
       </c>
       <c r="F37" s="9">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="G37" s="3">
         <f>E37*F37</f>
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" t="s">
         <v>203</v>
-      </c>
-      <c r="B38" t="s">
-        <v>206</v>
       </c>
       <c r="C38" t="s">
         <v>101</v>
@@ -2457,200 +2462,208 @@
         <v>0.09</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="0"/>
+        <f>E38*F38</f>
         <v>0.09</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" s="9">
-        <v>2.0699999999999998</v>
+        <v>0.09</v>
       </c>
       <c r="G39" s="3">
         <f t="shared" si="0"/>
-        <v>2.0699999999999998</v>
+        <v>0.09</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" t="s">
-        <v>123</v>
-      </c>
-      <c r="J39" t="s">
-        <v>120</v>
-      </c>
-      <c r="K39" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="I40" t="s">
+        <v>123</v>
+      </c>
+      <c r="J40" t="s">
+        <v>120</v>
+      </c>
+      <c r="K40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>125</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>126</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>127</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>127</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" s="9">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="9">
         <v>1.6</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G41" s="3">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H41" s="20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5">
-        <f>SUM(G4:G40)</f>
-        <v>60.796000000000014</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1" t="s">
+      <c r="G42" s="5">
+        <f>SUM(G4:G41)</f>
+        <v>61.336000000000013</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="3">
-        <v>2</v>
-      </c>
-      <c r="G44" s="3">
-        <f>F44*E44</f>
-        <v>2</v>
-      </c>
-      <c r="H44" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45" s="3">
-        <v>0.38</v>
+        <v>2</v>
       </c>
       <c r="G45" s="3">
         <f>F45*E45</f>
+        <v>2</v>
+      </c>
+      <c r="H45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>209</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
         <v>0.38</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="B46" s="15"/>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3">
-        <v>5.1100000000000003</v>
       </c>
       <c r="G46" s="3">
         <f>F46*E46</f>
+        <v>0.38</v>
+      </c>
+      <c r="H46" s="20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
         <v>5.1100000000000003</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="B47" s="12"/>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
-        <v>6.11</v>
       </c>
       <c r="G47" s="3">
         <f>F47*E47</f>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
         <v>6.11</v>
       </c>
-      <c r="H47" s="20" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>240</v>
-      </c>
-      <c r="B48" s="29"/>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1.22</v>
-      </c>
       <c r="G48" s="3">
-        <f t="shared" ref="G48:G50" si="1">F48*E48</f>
-        <v>2.44</v>
+        <f>F48*E48</f>
+        <v>6.11</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -2659,308 +2672,312 @@
         <v>1.22</v>
       </c>
       <c r="G49" s="3">
+        <f t="shared" ref="G49:G51" si="1">F49*E49</f>
+        <v>2.44</v>
+      </c>
+      <c r="H49" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>236</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="G50" s="3">
         <f t="shared" si="1"/>
         <v>2.44</v>
       </c>
-      <c r="H49" s="20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="H50" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>175</v>
       </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G51" s="3">
         <f t="shared" si="1"/>
         <v>2.0099999999999998</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H51" s="20" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G51" s="3">
-        <f t="shared" ref="G47:G57" si="2">F51*E51</f>
+      <c r="G52" s="3">
+        <f t="shared" ref="G52:G58" si="2">F52*E52</f>
         <v>2.4700000000000002</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H52" s="20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>154</v>
       </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="3">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
         <v>5</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G53" s="3">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>212</v>
       </c>
-      <c r="E53">
+      <c r="B54" t="s">
+        <v>211</v>
+      </c>
+      <c r="E54">
         <v>4</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F54" s="3">
         <v>0.1</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G54" s="3">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="H53" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="B54" t="s">
-        <v>224</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G54" s="3">
-        <f>F53*E53</f>
-        <v>0.4</v>
-      </c>
       <c r="H54" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>215</v>
+      <c r="A55" s="15" t="s">
+        <v>222</v>
       </c>
       <c r="B55" t="s">
+        <v>223</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G55" s="3">
+        <f>F54*E54</f>
+        <v>0.4</v>
+      </c>
+      <c r="H55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="E55">
+      <c r="B56" t="s">
+        <v>213</v>
+      </c>
+      <c r="E56">
         <v>4</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F56" s="3">
         <v>0.1</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G56" s="3">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57" t="s">
         <v>216</v>
       </c>
-      <c r="B56" t="s">
-        <v>217</v>
-      </c>
-      <c r="E56">
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F57" s="3">
         <v>0.1</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G57" s="3">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="H56" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-      <c r="G57" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
       <c r="H57" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="5">
-        <f>SUM(G44:G57)</f>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="5">
+        <f>SUM(G45:G58)</f>
         <v>30.359999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="24" t="s">
+    <row r="61" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="24"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>171.4</v>
+      </c>
+      <c r="G62">
+        <f>F62*E62</f>
+        <v>171.4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B64" s="24"/>
+      <c r="C64" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>224</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3">
+        <v>35.06</v>
+      </c>
+      <c r="G65">
+        <v>35.06</v>
+      </c>
+      <c r="H65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="B60" s="24"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>157</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="3">
-        <v>171.4</v>
-      </c>
-      <c r="G61">
-        <f>F61*E61</f>
-        <v>171.4</v>
-      </c>
-      <c r="H61" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D63" s="19"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>225</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64" s="3">
-        <v>35.06</v>
-      </c>
-      <c r="G64">
-        <v>35.06</v>
-      </c>
-      <c r="H64" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="B66" s="24"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>159</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67" s="3">
-        <v>66.34</v>
-      </c>
-      <c r="G67">
-        <f t="shared" ref="G67:G68" si="3">F67*E67</f>
-        <v>66.34</v>
-      </c>
-      <c r="H67" t="s">
-        <v>160</v>
-      </c>
+      <c r="B67" s="24"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>66.34</v>
+      </c>
+      <c r="G68">
+        <f t="shared" ref="G68:G69" si="3">F68*E68</f>
+        <v>66.34</v>
+      </c>
+      <c r="H68" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>162</v>
       </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68" s="3">
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
         <v>38.340000000000003</v>
       </c>
-      <c r="G68">
+      <c r="G69">
         <f t="shared" si="3"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H69" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G69" s="5">
-        <f>SUM(G67:G68)</f>
+      <c r="G70" s="5">
+        <f>SUM(G68:G69)</f>
         <v>104.68</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="23" t="s">
+    <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="23" t="s">
         <v>176</v>
-      </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="18">
-        <f>G69+G58+G41+G61</f>
-        <v>367.23599999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="23" t="s">
-        <v>231</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="23"/>
@@ -2968,31 +2985,45 @@
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
       <c r="G72" s="18">
-        <f>G69+G58+G41+G64</f>
-        <v>230.89600000000002</v>
+        <f>G70+G59+G42+G62</f>
+        <v>367.77600000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18">
+        <f>G70+G59+G42+G65</f>
+        <v>231.43600000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A71:C71"/>
     <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H60" r:id="rId6" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H64" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H61" r:id="rId8" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
-    <hyperlink ref="H7" r:id="rId9" xr:uid="{248762FA-4AB4-4C5B-BD9F-71361739AEC2}"/>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H29" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H61" r:id="rId6" display="https://www.aliexpress.com/item/1005005857983522.html" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H65" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H62" r:id="rId8" display="https://www.aliexpress.com/item/1005005736571669.html" xr:uid="{FFB216EB-1022-4E93-8DA0-1B15666E6B23}"/>
+    <hyperlink ref="H8" r:id="rId9" xr:uid="{248762FA-4AB4-4C5B-BD9F-71361739AEC2}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>

</xml_diff>